<commit_message>
fixed memory unit issues
</commit_message>
<xml_diff>
--- a/computerArchitecture/test/resources/test3/memory.xlsx
+++ b/computerArchitecture/test/resources/test3/memory.xlsx
@@ -954,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P202"/>
+    <sheetView tabSelected="1" topLeftCell="F88" workbookViewId="0">
+      <selection activeCell="P102" sqref="P102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,7 +2021,7 @@
         <v>16</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" ref="O14:O22" si="20">"00000000"</f>
+        <f t="shared" ref="O18:O22" si="20">"00000000"</f>
         <v>00000000</v>
       </c>
       <c r="P18" t="s">
@@ -3057,8 +3057,8 @@
         <v>CAFECAFE</v>
       </c>
       <c r="P102" t="str">
-        <f>"00000002"</f>
-        <v>00000002</v>
+        <f>"40000000"</f>
+        <v>40000000</v>
       </c>
     </row>
     <row r="103" spans="14:16" x14ac:dyDescent="0.25">

</xml_diff>